<commit_message>
change size text excel + print excel
</commit_message>
<xml_diff>
--- a/studMin/TemplateExcel/schedule_student.xlsx
+++ b/studMin/TemplateExcel/schedule_student.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Thiet\source\repos\studMin\studMin\TemplateExcel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2088EBC6-55C4-4D44-AABD-82F705F716E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{729C4C25-4BB3-4BF2-9DA1-89D313266B56}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="15945" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -74,7 +74,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -96,47 +96,41 @@
       <name val="Arial"/>
     </font>
     <font>
-      <sz val="10"/>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="13"/>
       <color theme="1"/>
       <name val="Times New Roman"/>
+      <family val="1"/>
     </font>
     <font>
       <b/>
-      <sz val="11"/>
+      <sz val="13"/>
       <color theme="1"/>
       <name val="Times New Roman"/>
+      <family val="1"/>
     </font>
     <font>
-      <b/>
-      <sz val="12"/>
-      <color theme="1"/>
-      <name val="Times New Roman"/>
+      <sz val="13"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="14"/>
       <color theme="1"/>
       <name val="Times New Roman"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color theme="1"/>
-      <name val="Times New Roman"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Times New Roman"/>
+      <family val="1"/>
+      <charset val="163"/>
     </font>
     <font>
       <sz val="14"/>
-      <color theme="1"/>
-      <name val="Times New Roman"/>
-    </font>
-    <font>
-      <sz val="14"/>
-      <color theme="1"/>
       <name val="Arial"/>
+      <family val="2"/>
+      <charset val="163"/>
     </font>
   </fonts>
   <fills count="7">
@@ -470,83 +464,83 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -769,7 +763,7 @@
   <dimension ref="A1:AD1003"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+      <selection activeCell="C2" sqref="C2:E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.3984375" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -779,16 +773,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:30" ht="30.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="14" t="s">
+      <c r="A1" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="15"/>
-      <c r="C1" s="15"/>
-      <c r="D1" s="15"/>
-      <c r="E1" s="15"/>
-      <c r="F1" s="15"/>
-      <c r="G1" s="15"/>
-      <c r="H1" s="16"/>
+      <c r="B1" s="17"/>
+      <c r="C1" s="17"/>
+      <c r="D1" s="17"/>
+      <c r="E1" s="17"/>
+      <c r="F1" s="17"/>
+      <c r="G1" s="17"/>
+      <c r="H1" s="18"/>
       <c r="I1" s="1"/>
       <c r="J1" s="1"/>
       <c r="K1" s="1"/>
@@ -812,19 +806,19 @@
       <c r="AC1" s="1"/>
       <c r="AD1" s="1"/>
     </row>
-    <row r="2" spans="1:30" ht="13.5" x14ac:dyDescent="0.35">
-      <c r="A2" s="2"/>
-      <c r="B2" s="2"/>
-      <c r="C2" s="3" t="s">
+    <row r="2" spans="1:30" ht="17.25" x14ac:dyDescent="0.45">
+      <c r="A2" s="3"/>
+      <c r="B2" s="3"/>
+      <c r="C2" s="27" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="17" t="s">
+      <c r="D2" s="28" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="18"/>
-      <c r="F2" s="2"/>
-      <c r="G2" s="2"/>
-      <c r="H2" s="2"/>
+      <c r="E2" s="29"/>
+      <c r="F2" s="3"/>
+      <c r="G2" s="3"/>
+      <c r="H2" s="3"/>
       <c r="I2" s="1"/>
       <c r="J2" s="1"/>
       <c r="K2" s="1"/>
@@ -848,21 +842,21 @@
       <c r="AC2" s="1"/>
       <c r="AD2" s="1"/>
     </row>
-    <row r="3" spans="1:30" ht="13.5" x14ac:dyDescent="0.35">
-      <c r="A3" s="2"/>
-      <c r="B3" s="2"/>
-      <c r="C3" s="4" t="s">
+    <row r="3" spans="1:30" ht="17.25" x14ac:dyDescent="0.35">
+      <c r="A3" s="3"/>
+      <c r="B3" s="3"/>
+      <c r="C3" s="30" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="5" t="s">
+      <c r="D3" s="31" t="s">
         <v>4</v>
       </c>
-      <c r="E3" s="6" t="s">
+      <c r="E3" s="32" t="s">
         <v>5</v>
       </c>
-      <c r="F3" s="2"/>
-      <c r="G3" s="2"/>
-      <c r="H3" s="2"/>
+      <c r="F3" s="3"/>
+      <c r="G3" s="3"/>
+      <c r="H3" s="3"/>
       <c r="I3" s="1"/>
       <c r="J3" s="1"/>
       <c r="K3" s="1"/>
@@ -886,15 +880,15 @@
       <c r="AC3" s="1"/>
       <c r="AD3" s="1"/>
     </row>
-    <row r="4" spans="1:30" ht="13.15" x14ac:dyDescent="0.35">
-      <c r="A4" s="7"/>
-      <c r="B4" s="7"/>
-      <c r="C4" s="7"/>
-      <c r="D4" s="7"/>
-      <c r="E4" s="7"/>
-      <c r="F4" s="7"/>
-      <c r="G4" s="7"/>
-      <c r="H4" s="7"/>
+    <row r="4" spans="1:30" ht="16.5" x14ac:dyDescent="0.35">
+      <c r="A4" s="4"/>
+      <c r="B4" s="4"/>
+      <c r="C4" s="4"/>
+      <c r="D4" s="4"/>
+      <c r="E4" s="4"/>
+      <c r="F4" s="4"/>
+      <c r="G4" s="4"/>
+      <c r="H4" s="4"/>
       <c r="I4" s="1"/>
       <c r="J4" s="1"/>
       <c r="K4" s="1"/>
@@ -918,29 +912,29 @@
       <c r="AC4" s="1"/>
       <c r="AD4" s="1"/>
     </row>
-    <row r="5" spans="1:30" ht="17.25" x14ac:dyDescent="0.35">
-      <c r="A5" s="8" t="s">
+    <row r="5" spans="1:30" ht="16.5" x14ac:dyDescent="0.35">
+      <c r="A5" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="8" t="s">
+      <c r="B5" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="9" t="s">
+      <c r="C5" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="D5" s="9" t="s">
+      <c r="D5" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="E5" s="9" t="s">
+      <c r="E5" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="F5" s="9" t="s">
+      <c r="F5" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="G5" s="9" t="s">
+      <c r="G5" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="H5" s="9" t="s">
+      <c r="H5" s="6" t="s">
         <v>13</v>
       </c>
       <c r="I5" s="1"/>
@@ -966,19 +960,19 @@
       <c r="AC5" s="1"/>
       <c r="AD5" s="1"/>
     </row>
-    <row r="6" spans="1:30" ht="15.4" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:30" ht="16.5" x14ac:dyDescent="0.35">
       <c r="A6" s="19" t="s">
         <v>14</v>
       </c>
-      <c r="B6" s="10">
+      <c r="B6" s="7">
         <v>1</v>
       </c>
-      <c r="C6" s="28"/>
-      <c r="D6" s="29"/>
-      <c r="E6" s="29"/>
-      <c r="F6" s="29"/>
-      <c r="G6" s="29"/>
-      <c r="H6" s="29"/>
+      <c r="C6" s="8"/>
+      <c r="D6" s="9"/>
+      <c r="E6" s="9"/>
+      <c r="F6" s="9"/>
+      <c r="G6" s="9"/>
+      <c r="H6" s="9"/>
       <c r="I6" s="1"/>
       <c r="J6" s="1"/>
       <c r="K6" s="1"/>
@@ -1002,17 +996,17 @@
       <c r="AC6" s="1"/>
       <c r="AD6" s="1"/>
     </row>
-    <row r="7" spans="1:30" ht="15.4" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:30" ht="16.5" x14ac:dyDescent="0.35">
       <c r="A7" s="20"/>
-      <c r="B7" s="11">
+      <c r="B7" s="10">
         <v>2</v>
       </c>
-      <c r="C7" s="28"/>
-      <c r="D7" s="29"/>
-      <c r="E7" s="29"/>
-      <c r="F7" s="29"/>
-      <c r="G7" s="29"/>
-      <c r="H7" s="29"/>
+      <c r="C7" s="8"/>
+      <c r="D7" s="9"/>
+      <c r="E7" s="9"/>
+      <c r="F7" s="9"/>
+      <c r="G7" s="9"/>
+      <c r="H7" s="9"/>
       <c r="I7" s="1"/>
       <c r="J7" s="1"/>
       <c r="K7" s="1"/>
@@ -1036,17 +1030,17 @@
       <c r="AC7" s="1"/>
       <c r="AD7" s="1"/>
     </row>
-    <row r="8" spans="1:30" ht="15.4" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:30" ht="16.5" x14ac:dyDescent="0.35">
       <c r="A8" s="20"/>
-      <c r="B8" s="11">
+      <c r="B8" s="10">
         <v>3</v>
       </c>
-      <c r="C8" s="28"/>
-      <c r="D8" s="29"/>
-      <c r="E8" s="29"/>
-      <c r="F8" s="29"/>
-      <c r="G8" s="29"/>
-      <c r="H8" s="29"/>
+      <c r="C8" s="8"/>
+      <c r="D8" s="9"/>
+      <c r="E8" s="9"/>
+      <c r="F8" s="9"/>
+      <c r="G8" s="9"/>
+      <c r="H8" s="9"/>
       <c r="I8" s="1"/>
       <c r="J8" s="1"/>
       <c r="K8" s="1"/>
@@ -1070,17 +1064,17 @@
       <c r="AC8" s="1"/>
       <c r="AD8" s="1"/>
     </row>
-    <row r="9" spans="1:30" ht="15.4" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:30" ht="16.5" x14ac:dyDescent="0.35">
       <c r="A9" s="20"/>
-      <c r="B9" s="11">
+      <c r="B9" s="10">
         <v>4</v>
       </c>
-      <c r="C9" s="28"/>
-      <c r="D9" s="29"/>
-      <c r="E9" s="29"/>
-      <c r="F9" s="29"/>
-      <c r="G9" s="29"/>
-      <c r="H9" s="29"/>
+      <c r="C9" s="8"/>
+      <c r="D9" s="9"/>
+      <c r="E9" s="9"/>
+      <c r="F9" s="9"/>
+      <c r="G9" s="9"/>
+      <c r="H9" s="9"/>
       <c r="I9" s="1"/>
       <c r="J9" s="1"/>
       <c r="K9" s="1"/>
@@ -1104,17 +1098,17 @@
       <c r="AC9" s="1"/>
       <c r="AD9" s="1"/>
     </row>
-    <row r="10" spans="1:30" ht="15.4" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:30" ht="16.5" x14ac:dyDescent="0.35">
       <c r="A10" s="21"/>
-      <c r="B10" s="11">
+      <c r="B10" s="10">
         <v>5</v>
       </c>
-      <c r="C10" s="32"/>
-      <c r="D10" s="32"/>
-      <c r="E10" s="32"/>
-      <c r="F10" s="32"/>
-      <c r="G10" s="32"/>
-      <c r="H10" s="32"/>
+      <c r="C10" s="11"/>
+      <c r="D10" s="11"/>
+      <c r="E10" s="11"/>
+      <c r="F10" s="11"/>
+      <c r="G10" s="11"/>
+      <c r="H10" s="11"/>
       <c r="I10" s="1"/>
       <c r="J10" s="1"/>
       <c r="K10" s="1"/>
@@ -1170,19 +1164,19 @@
       <c r="AC11" s="1"/>
       <c r="AD11" s="1"/>
     </row>
-    <row r="12" spans="1:30" ht="15.4" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:30" ht="16.5" x14ac:dyDescent="0.35">
       <c r="A12" s="22" t="s">
         <v>15</v>
       </c>
-      <c r="B12" s="11">
+      <c r="B12" s="10">
         <v>1</v>
       </c>
-      <c r="C12" s="27"/>
-      <c r="D12" s="27"/>
-      <c r="E12" s="27"/>
-      <c r="F12" s="27"/>
-      <c r="G12" s="27"/>
-      <c r="H12" s="27"/>
+      <c r="C12" s="12"/>
+      <c r="D12" s="12"/>
+      <c r="E12" s="12"/>
+      <c r="F12" s="12"/>
+      <c r="G12" s="12"/>
+      <c r="H12" s="12"/>
       <c r="I12" s="1"/>
       <c r="J12" s="1"/>
       <c r="K12" s="1"/>
@@ -1206,17 +1200,17 @@
       <c r="AC12" s="1"/>
       <c r="AD12" s="1"/>
     </row>
-    <row r="13" spans="1:30" ht="15.4" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:30" ht="16.5" x14ac:dyDescent="0.35">
       <c r="A13" s="20"/>
-      <c r="B13" s="11">
+      <c r="B13" s="10">
         <v>2</v>
       </c>
-      <c r="C13" s="28"/>
-      <c r="D13" s="29"/>
-      <c r="E13" s="29"/>
-      <c r="F13" s="29"/>
-      <c r="G13" s="29"/>
-      <c r="H13" s="29"/>
+      <c r="C13" s="8"/>
+      <c r="D13" s="9"/>
+      <c r="E13" s="9"/>
+      <c r="F13" s="9"/>
+      <c r="G13" s="9"/>
+      <c r="H13" s="9"/>
       <c r="I13" s="1"/>
       <c r="J13" s="1"/>
       <c r="K13" s="1"/>
@@ -1240,17 +1234,17 @@
       <c r="AC13" s="1"/>
       <c r="AD13" s="1"/>
     </row>
-    <row r="14" spans="1:30" ht="15.4" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:30" ht="16.5" x14ac:dyDescent="0.35">
       <c r="A14" s="20"/>
-      <c r="B14" s="11">
+      <c r="B14" s="10">
         <v>3</v>
       </c>
-      <c r="C14" s="28"/>
-      <c r="D14" s="29"/>
-      <c r="E14" s="29"/>
-      <c r="F14" s="29"/>
-      <c r="G14" s="29"/>
-      <c r="H14" s="29"/>
+      <c r="C14" s="8"/>
+      <c r="D14" s="9"/>
+      <c r="E14" s="9"/>
+      <c r="F14" s="9"/>
+      <c r="G14" s="9"/>
+      <c r="H14" s="9"/>
       <c r="I14" s="1"/>
       <c r="J14" s="1"/>
       <c r="K14" s="1"/>
@@ -1274,17 +1268,17 @@
       <c r="AC14" s="1"/>
       <c r="AD14" s="1"/>
     </row>
-    <row r="15" spans="1:30" ht="15.4" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:30" ht="16.5" x14ac:dyDescent="0.35">
       <c r="A15" s="20"/>
-      <c r="B15" s="11">
+      <c r="B15" s="10">
         <v>4</v>
       </c>
-      <c r="C15" s="28"/>
-      <c r="D15" s="29"/>
-      <c r="E15" s="29"/>
-      <c r="F15" s="29"/>
-      <c r="G15" s="29"/>
-      <c r="H15" s="29"/>
+      <c r="C15" s="8"/>
+      <c r="D15" s="9"/>
+      <c r="E15" s="9"/>
+      <c r="F15" s="9"/>
+      <c r="G15" s="9"/>
+      <c r="H15" s="9"/>
       <c r="I15" s="1"/>
       <c r="J15" s="1"/>
       <c r="K15" s="1"/>
@@ -1308,17 +1302,17 @@
       <c r="AC15" s="1"/>
       <c r="AD15" s="1"/>
     </row>
-    <row r="16" spans="1:30" ht="15.4" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:30" ht="16.5" x14ac:dyDescent="0.35">
       <c r="A16" s="23"/>
-      <c r="B16" s="12">
+      <c r="B16" s="13">
         <v>5</v>
       </c>
-      <c r="C16" s="30"/>
-      <c r="D16" s="31"/>
-      <c r="E16" s="31"/>
-      <c r="F16" s="31"/>
-      <c r="G16" s="31"/>
-      <c r="H16" s="31"/>
+      <c r="C16" s="14"/>
+      <c r="D16" s="15"/>
+      <c r="E16" s="15"/>
+      <c r="F16" s="15"/>
+      <c r="G16" s="15"/>
+      <c r="H16" s="15"/>
       <c r="I16" s="1"/>
       <c r="J16" s="1"/>
       <c r="K16" s="1"/>
@@ -1345,12 +1339,12 @@
     <row r="17" spans="1:30" ht="17.25" x14ac:dyDescent="0.35">
       <c r="A17" s="1"/>
       <c r="B17" s="1"/>
-      <c r="C17" s="13"/>
-      <c r="D17" s="13"/>
-      <c r="E17" s="13"/>
-      <c r="F17" s="13"/>
-      <c r="G17" s="13"/>
-      <c r="H17" s="13"/>
+      <c r="C17" s="2"/>
+      <c r="D17" s="2"/>
+      <c r="E17" s="2"/>
+      <c r="F17" s="2"/>
+      <c r="G17" s="2"/>
+      <c r="H17" s="2"/>
       <c r="I17" s="1"/>
       <c r="J17" s="1"/>
       <c r="K17" s="1"/>
@@ -32935,5 +32929,6 @@
     <mergeCell ref="A11:H11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>